<commit_message>
static, switches 폴더 > 0614 버전
</commit_message>
<xml_diff>
--- a/static/form.xlsx
+++ b/static/form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daery\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이대리\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,26 +212,32 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,48 +523,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="5" customWidth="1"/>
-    <col min="2" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="7" customWidth="1"/>
+    <col min="2" max="3" width="12.5" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>